<commit_message>
Finished results and had a couple of code changes
</commit_message>
<xml_diff>
--- a/AlgorithmsProject1/results.xlsx
+++ b/AlgorithmsProject1/results.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="10 Runs, 100,000 Elems" sheetId="1" r:id="rId1"/>
     <sheet name="100 Runs, 100,000 Elems" sheetId="2" r:id="rId2"/>
     <sheet name="10 Runs, 10,000 Elems" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
   <si>
     <t>10,000 Range</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -555,8 +558,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -982,11 +988,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="374303120"/>
-        <c:axId val="374303512"/>
+        <c:axId val="273147624"/>
+        <c:axId val="273146840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374303120"/>
+        <c:axId val="273147624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374303512"/>
+        <c:crossAx val="273146840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1037,7 +1043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374303512"/>
+        <c:axId val="273146840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374303120"/>
+        <c:crossAx val="273147624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1537,11 +1543,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="374941528"/>
-        <c:axId val="374939960"/>
+        <c:axId val="275082160"/>
+        <c:axId val="275085688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374941528"/>
+        <c:axId val="275082160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1590,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374939960"/>
+        <c:crossAx val="275085688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1592,7 +1598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374939960"/>
+        <c:axId val="275085688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1643,7 +1649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374941528"/>
+        <c:crossAx val="275082160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2088,11 +2094,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="108994096"/>
-        <c:axId val="493811696"/>
+        <c:axId val="275084512"/>
+        <c:axId val="275081768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108994096"/>
+        <c:axId val="275084512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2135,7 +2141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493811696"/>
+        <c:crossAx val="275081768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2143,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="493811696"/>
+        <c:axId val="275081768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108994096"/>
+        <c:crossAx val="275084512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2632,11 +2638,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="493804640"/>
-        <c:axId val="493810520"/>
+        <c:axId val="275086080"/>
+        <c:axId val="275086864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="493804640"/>
+        <c:axId val="275086080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2679,7 +2685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493810520"/>
+        <c:crossAx val="275086864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2687,7 +2693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="493810520"/>
+        <c:axId val="275086864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,7 +2744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493804640"/>
+        <c:crossAx val="275086080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3180,11 +3186,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="111816976"/>
-        <c:axId val="111817760"/>
+        <c:axId val="275086472"/>
+        <c:axId val="275087256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111816976"/>
+        <c:axId val="275086472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3227,7 +3233,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111817760"/>
+        <c:crossAx val="275087256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3235,7 +3241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111817760"/>
+        <c:axId val="275087256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3286,7 +3292,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111816976"/>
+        <c:crossAx val="275086472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3728,11 +3734,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="111819720"/>
-        <c:axId val="488083880"/>
+        <c:axId val="275087648"/>
+        <c:axId val="275080592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="111819720"/>
+        <c:axId val="275087648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3775,7 +3781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488083880"/>
+        <c:crossAx val="275080592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3783,7 +3789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488083880"/>
+        <c:axId val="275080592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,7 +3840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111819720"/>
+        <c:crossAx val="275087648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4272,11 +4278,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="488079960"/>
-        <c:axId val="488089368"/>
+        <c:axId val="275080984"/>
+        <c:axId val="275085296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="488079960"/>
+        <c:axId val="275080984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,7 +4325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488089368"/>
+        <c:crossAx val="275085296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4327,7 +4333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="488089368"/>
+        <c:axId val="275085296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4378,7 +4384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="488079960"/>
+        <c:crossAx val="275080984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4827,11 +4833,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="376155600"/>
-        <c:axId val="376156384"/>
+        <c:axId val="275084904"/>
+        <c:axId val="275081376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="376155600"/>
+        <c:axId val="275084904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4874,7 +4880,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376156384"/>
+        <c:crossAx val="275081376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4882,7 +4888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376156384"/>
+        <c:axId val="275081376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4933,7 +4939,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376155600"/>
+        <c:crossAx val="275084904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5378,11 +5384,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="376153248"/>
-        <c:axId val="376153640"/>
+        <c:axId val="144977192"/>
+        <c:axId val="144977584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="376153248"/>
+        <c:axId val="144977192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5425,7 +5431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376153640"/>
+        <c:crossAx val="144977584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5433,7 +5439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376153640"/>
+        <c:axId val="144977584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5484,7 +5490,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376153248"/>
+        <c:crossAx val="144977192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5922,11 +5928,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="487396648"/>
-        <c:axId val="487393904"/>
+        <c:axId val="144978368"/>
+        <c:axId val="144978760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="487396648"/>
+        <c:axId val="144978368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5969,7 +5975,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487393904"/>
+        <c:crossAx val="144978760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5977,7 +5983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="487393904"/>
+        <c:axId val="144978760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6028,7 +6034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487396648"/>
+        <c:crossAx val="144978368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6195,7 +6201,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$E$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6248,7 +6254,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$E$3:$E$9,'10 Runs, 100,000 Elems'!$E$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$F$3:$F$9,'10 Runs, 100,000 Elems'!$F$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6285,7 +6291,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$F$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6338,7 +6344,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$F$3:$F$9,'10 Runs, 100,000 Elems'!$F$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$G$3:$G$9,'10 Runs, 100,000 Elems'!$G$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6375,7 +6381,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$G$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6428,7 +6434,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$G$3:$G$9,'10 Runs, 100,000 Elems'!$G$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$H$3:$H$9,'10 Runs, 100,000 Elems'!$H$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6470,11 +6476,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="374305864"/>
-        <c:axId val="374298808"/>
+        <c:axId val="273145272"/>
+        <c:axId val="273146056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374305864"/>
+        <c:axId val="273145272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6517,7 +6523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374298808"/>
+        <c:crossAx val="273146056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6525,7 +6531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374298808"/>
+        <c:axId val="273146056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6576,7 +6582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374305864"/>
+        <c:crossAx val="273145272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6739,7 +6745,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$H$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6792,7 +6798,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$H$3:$H$9,'10 Runs, 100,000 Elems'!$H$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$J$3:$J$9,'10 Runs, 100,000 Elems'!$J$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6829,7 +6835,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$I$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6882,7 +6888,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$I$3:$I$9,'10 Runs, 100,000 Elems'!$I$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$K$3:$K$9,'10 Runs, 100,000 Elems'!$K$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6919,7 +6925,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$J$2</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6972,7 +6978,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$J$3:$J$9,'10 Runs, 100,000 Elems'!$J$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$L$3:$L$9,'10 Runs, 100,000 Elems'!$L$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7014,11 +7020,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="374306256"/>
-        <c:axId val="374299592"/>
+        <c:axId val="273144488"/>
+        <c:axId val="274239576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374306256"/>
+        <c:axId val="273144488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7061,7 +7067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374299592"/>
+        <c:crossAx val="274239576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7069,7 +7075,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374299592"/>
+        <c:axId val="274239576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7120,7 +7126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374306256"/>
+        <c:crossAx val="273144488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7384,7 +7390,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$E$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7437,7 +7443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$E$3:$E$9,'10 Runs, 100,000 Elems'!$E$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$F$3:$F$9,'10 Runs, 100,000 Elems'!$F$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7474,7 +7480,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$H$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7527,7 +7533,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$H$3:$H$9,'10 Runs, 100,000 Elems'!$H$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$J$3:$J$9,'10 Runs, 100,000 Elems'!$J$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7569,11 +7575,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="42950288"/>
-        <c:axId val="482908800"/>
+        <c:axId val="274240360"/>
+        <c:axId val="274242712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42950288"/>
+        <c:axId val="274240360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7616,7 +7622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482908800"/>
+        <c:crossAx val="274242712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7624,7 +7630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482908800"/>
+        <c:axId val="274242712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7675,7 +7681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42950288"/>
+        <c:crossAx val="274240360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7935,7 +7941,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$E$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7988,7 +7994,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$F$3:$F$9,'10 Runs, 100,000 Elems'!$F$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$G$3:$G$9,'10 Runs, 100,000 Elems'!$G$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8025,7 +8031,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$H$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8078,7 +8084,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$I$3:$I$9,'10 Runs, 100,000 Elems'!$I$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$K$3:$K$9,'10 Runs, 100,000 Elems'!$K$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8120,11 +8126,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="487397432"/>
-        <c:axId val="487391552"/>
+        <c:axId val="274241144"/>
+        <c:axId val="274235656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="487397432"/>
+        <c:axId val="274241144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8167,7 +8173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487391552"/>
+        <c:crossAx val="274235656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8175,7 +8181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="487391552"/>
+        <c:axId val="274235656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8226,7 +8232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487397432"/>
+        <c:crossAx val="274241144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8479,7 +8485,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$E$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8532,7 +8538,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$G$3:$G$9,'10 Runs, 100,000 Elems'!$G$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$H$3:$H$9,'10 Runs, 100,000 Elems'!$H$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8569,7 +8575,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'10 Runs, 100,000 Elems'!$H$1</c:f>
+              <c:f>'10 Runs, 100,000 Elems'!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8622,7 +8628,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('10 Runs, 100,000 Elems'!$J$3:$J$9,'10 Runs, 100,000 Elems'!$J$11)</c:f>
+              <c:f>('10 Runs, 100,000 Elems'!$L$3:$L$9,'10 Runs, 100,000 Elems'!$L$11)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8664,11 +8670,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="376154032"/>
-        <c:axId val="376154816"/>
+        <c:axId val="274241928"/>
+        <c:axId val="274242320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="376154032"/>
+        <c:axId val="274241928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8711,7 +8717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376154816"/>
+        <c:crossAx val="274242320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8719,7 +8725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376154816"/>
+        <c:axId val="274242320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8770,7 +8776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376154032"/>
+        <c:crossAx val="274241928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9212,11 +9218,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="482911152"/>
-        <c:axId val="482913504"/>
+        <c:axId val="274239184"/>
+        <c:axId val="274243104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482911152"/>
+        <c:axId val="274239184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9259,7 +9265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482913504"/>
+        <c:crossAx val="274243104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9267,7 +9273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482913504"/>
+        <c:axId val="274243104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9318,7 +9324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482911152"/>
+        <c:crossAx val="274239184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9760,11 +9766,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="376151680"/>
-        <c:axId val="376155992"/>
+        <c:axId val="274236048"/>
+        <c:axId val="274236832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="376151680"/>
+        <c:axId val="274236048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9807,7 +9813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376155992"/>
+        <c:crossAx val="274236832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9815,7 +9821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="376155992"/>
+        <c:axId val="274236832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9866,7 +9872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376151680"/>
+        <c:crossAx val="274236048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10304,11 +10310,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="376149328"/>
-        <c:axId val="487393120"/>
+        <c:axId val="274237616"/>
+        <c:axId val="274238008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="376149328"/>
+        <c:axId val="274237616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10351,7 +10357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="487393120"/>
+        <c:crossAx val="274238008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10359,7 +10365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="487393120"/>
+        <c:axId val="274238008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10410,7 +10416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376149328"/>
+        <c:crossAx val="274237616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20275,7 +20281,7 @@
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
@@ -20299,13 +20305,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>395287</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
@@ -20329,13 +20335,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>233362</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
@@ -20365,7 +20371,7 @@
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
@@ -20389,13 +20395,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>404812</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
@@ -20419,13 +20425,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>242887</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
@@ -21107,10 +21113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21118,24 +21124,27 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -21145,26 +21154,35 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -21178,28 +21196,37 @@
         <v>20</v>
       </c>
       <c r="E3">
+        <f>D3-C3</f>
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>11</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <f>H3-G3</f>
+        <v>4</v>
+      </c>
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>7</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
+      <c r="M3">
+        <f>L3-K3</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -21213,28 +21240,37 @@
         <v>12</v>
       </c>
       <c r="E4">
+        <f t="shared" ref="E4:E11" si="0">D4-C4</f>
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>9</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>11</v>
       </c>
-      <c r="H4">
+      <c r="I4">
+        <f t="shared" ref="I4:I11" si="1">H4-G4</f>
+        <v>3</v>
+      </c>
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>7</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
-        <v>7</v>
+      <c r="M4">
+        <f t="shared" ref="M4:M11" si="2">L4-K4</f>
+        <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -21248,28 +21284,37 @@
         <v>10</v>
       </c>
       <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>12</v>
       </c>
-      <c r="H5">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J5">
         <v>8</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>7</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>11</v>
       </c>
-      <c r="K5" t="s">
-        <v>7</v>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -21283,28 +21328,37 @@
         <v>11</v>
       </c>
       <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>11</v>
       </c>
-      <c r="H6">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J6">
         <v>8</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>7</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>11</v>
       </c>
-      <c r="K6" t="s">
-        <v>7</v>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -21318,28 +21372,37 @@
         <v>15</v>
       </c>
       <c r="E7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F7">
         <v>8</v>
       </c>
       <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="H7">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>8</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>8</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>10</v>
       </c>
-      <c r="K7" t="s">
-        <v>7</v>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -21353,28 +21416,37 @@
         <v>16</v>
       </c>
       <c r="E8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>9</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>13</v>
       </c>
-      <c r="H8">
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8">
         <v>10</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>9</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>13</v>
       </c>
-      <c r="K8" t="s">
-        <v>7</v>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -21388,28 +21460,37 @@
         <v>19</v>
       </c>
       <c r="E9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F9">
         <v>11</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>15</v>
       </c>
-      <c r="H9">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9">
         <v>10</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>13</v>
       </c>
-      <c r="K9" t="s">
-        <v>7</v>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -21423,28 +21504,37 @@
         <v>3254</v>
       </c>
       <c r="E10">
+        <f t="shared" si="0"/>
+        <v>324</v>
+      </c>
+      <c r="F10">
         <v>3225</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2934</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3723</v>
       </c>
-      <c r="H10">
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>789</v>
+      </c>
+      <c r="J10">
         <v>3165</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>2976</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>3604</v>
       </c>
-      <c r="K10" t="s">
-        <v>7</v>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>628</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -21458,37 +21548,46 @@
         <v>35</v>
       </c>
       <c r="E11">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F11">
         <v>7</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>9</v>
       </c>
-      <c r="H11">
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J11">
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>6</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>8</v>
       </c>
-      <c r="K11" t="s">
-        <v>7</v>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="30" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U30" t="s">
+    <row r="30" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W30" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21509,21 +21608,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -21884,8 +21983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21894,21 +21993,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">

</xml_diff>